<commit_message>
Orthorhombic reimplementation and updates to MI templating
</commit_message>
<xml_diff>
--- a/data/GroupSpec_rhombohedral.xlsx
+++ b/data/GroupSpec_rhombohedral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553C7E01-D91E-4645-86F7-7B5D13A504C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4514EEC9-CF89-1F4C-8BD4-D8EC15EA978D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2260" yWindow="-19640" windowWidth="27640" windowHeight="16940" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
+    <workbookView xWindow="140" yWindow="1000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FEA554-DCE4-B94D-8A39-A08CC83ACBDF}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10FA5DA-CE26-C14A-A284-A3F3DFB10698}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,7 +692,7 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>1315</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
         <v>20</v>
       </c>
       <c r="D3">
-        <v>5624</v>
+        <v>5567</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -748,13 +748,13 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>1520</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D7">
         <f>SUM(D2:D6)</f>
-        <v>9311</v>
+        <v>9187</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>21</v>
       </c>
       <c r="D9">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -800,7 +800,7 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <v>1674</v>
+        <v>1653</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -824,7 +824,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D11">
         <f>SUM(D9:D10)</f>
-        <v>2481</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>